<commit_message>
Update zutnlp-entity  2019-7-17 11:34:32
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>浅入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上午08:00-11:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初步完成zutnlp-entity后端</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -425,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -515,6 +527,20 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>43663</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update log  2019-7-17 21:49:13
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,6 +106,26 @@
   </si>
   <si>
     <t>完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下午14:00-18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初步学习发布部署服务器上的项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>了解实体关系抽取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浅入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浅入</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -437,17 +457,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.25" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
@@ -541,6 +561,28 @@
         <v>21</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>